<commit_message>
multiple wanted string option added
</commit_message>
<xml_diff>
--- a/Text-Extraction-Result.xlsx
+++ b/Text-Extraction-Result.xlsx
@@ -434,44 +434,53 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>File Name</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>File Name</t>
+          <t>Toplam Katma Değer Vergisi</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Value</t>
+          <t>Matrah Toplamı</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Örnek KDV Beyannamesi II.pdf</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Örnek KDV Beyannamesi II.pdf</t>
+          <t>113.122.268,06</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>113.122.268,06</t>
+          <t>2.936.636,47</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Örnek KDV Beyannamesi.pdf</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Örnek KDV Beyannamesi.pdf</t>
+          <t>565.316.718,40</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2.936.636,47</t>
+          <t>14.683.182,35</t>
         </is>
       </c>
     </row>

</xml_diff>